<commit_message>
Last version of Tempelates
</commit_message>
<xml_diff>
--- a/Templates-V2/Heat_and_Steam.xlsx
+++ b/Templates-V2/Heat_and_Steam.xlsx
@@ -5,11 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LevelupESG\Scope 2\Templates without to - from\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahmo\OneDrive\Desktop\Scope2\Batch-input-Page-main\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F30DE1-BF28-4B1E-9422-57BCF50D3AF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="CHyPYyhZlwlLm5OVvjxJ5wCg1DD6bMhfcEIwGuvdo2iaR4uGTpfKZ6UpyfsunWIP13Ldl9fkuPcmNz1+7rDqQA==" workbookSaltValue="XnmknF/4tG+vne+R2pJ7AQ==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B985273-788D-4CC3-844C-14CFF2080A98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{F659E81F-1463-40EE-92D2-40C09344B5C7}"/>
   </bookViews>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="168">
   <si>
     <t>Asset Name</t>
   </si>
@@ -499,9 +498,6 @@
     <t>ZWD</t>
   </si>
   <si>
-    <t>estimated</t>
-  </si>
-  <si>
     <t>The fiscal year for which the data is being reported, e.g., 2021</t>
   </si>
   <si>
@@ -532,16 +528,16 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>company1</t>
-  </si>
-  <si>
-    <t>reason 1</t>
-  </si>
-  <si>
-    <t>company2</t>
-  </si>
-  <si>
-    <t>reason 2</t>
+    <t>From</t>
+  </si>
+  <si>
+    <t>To</t>
+  </si>
+  <si>
+    <t>Starting date</t>
+  </si>
+  <si>
+    <t>Ending date</t>
   </si>
   <si>
     <t>Consumption</t>
@@ -619,7 +615,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -669,11 +665,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF8EA9DB"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -706,6 +711,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -714,7 +725,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="18">
     <dxf>
       <font>
         <color theme="2" tint="-0.499984740745262"/>
@@ -754,6 +765,12 @@
           <bgColor theme="2" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -852,18 +869,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{56746044-E903-4DB1-9F33-A53F32F0769F}" name="Table1" displayName="Table1" ref="A1:I1048576" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="14" tableBorderDxfId="13">
-  <autoFilter ref="A1:I1048576" xr:uid="{56746044-E903-4DB1-9F33-A53F32F0769F}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{9DF3A374-131F-43B6-9C39-C775FD7A98A5}" name="Asset Name" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{979BFCB7-7060-4B72-BBD7-A782ABC94E77}" name="Reporting Year" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{A2C51EF0-723B-4C20-A235-2C621CE89D87}" name="Value Type" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{C6DC634F-BE90-405E-BD48-D59C49E831A6}" name="Consumption (kWh)" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{A27BE819-CED3-47A8-9E36-A58D5807A455}" name="Typology" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{1748C08D-AF86-4EE8-9C7E-87CEAE19F1AD}" name="Total Spend" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{533AE4F7-857C-45AA-A9BD-1EC5B97FE058}" name="Currency " dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{FCA8F460-9AE1-4AB7-8E80-35EB816AB9DB}" name="Actual/Estimated" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{DD668173-3319-4CAD-9D50-7A3BF0641F5E}" name="Assumption basis" dataDxfId="4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{56746044-E903-4DB1-9F33-A53F32F0769F}" name="Table1" displayName="Table1" ref="A1:K1048574" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15">
+  <autoFilter ref="A1:K1048574" xr:uid="{56746044-E903-4DB1-9F33-A53F32F0769F}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{9DF3A374-131F-43B6-9C39-C775FD7A98A5}" name="Asset Name" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{979BFCB7-7060-4B72-BBD7-A782ABC94E77}" name="Reporting Year" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{A2C51EF0-723B-4C20-A235-2C621CE89D87}" name="Value Type" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{C6DC634F-BE90-405E-BD48-D59C49E831A6}" name="Consumption (kWh)" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{A27BE819-CED3-47A8-9E36-A58D5807A455}" name="Typology" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{1748C08D-AF86-4EE8-9C7E-87CEAE19F1AD}" name="Total Spend" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{533AE4F7-857C-45AA-A9BD-1EC5B97FE058}" name="Currency " dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{FCA8F460-9AE1-4AB7-8E80-35EB816AB9DB}" name="Actual/Estimated" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{DD668173-3319-4CAD-9D50-7A3BF0641F5E}" name="Assumption basis" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{0BFC6D8E-FC9C-477D-A300-E723BEC5A987}" name="From" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{3ADD3457-9EC1-48D7-B97C-04D74555F80F}" name="To" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1186,10 +1205,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D775E0E9-E192-457C-A3B8-47F95293021D}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:K1048576"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1200,13 +1219,15 @@
     <col min="4" max="4" width="20.6640625" style="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.88671875" style="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.77734375" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.77734375" style="15" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.33203125" style="9" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1"/>
+    <col min="10" max="10" width="12" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.77734375" style="9" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1234,45 +1255,57 @@
       <c r="I1" s="10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="J1" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="D2" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="E2" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="F2" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="G2" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="H2" s="12" t="s">
         <v>159</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="I2" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="J2" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>161</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>162</v>
       </c>
       <c r="B3" s="1">
         <v>2023</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D3" s="1">
         <v>1000</v>
@@ -1286,58 +1319,17 @@
         <v>11</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B4" s="1">
-        <v>2023</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="1">
-        <v>30</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="B5" s="9">
-        <v>2023</v>
-      </c>
-      <c r="D5" s="9">
-        <v>30</v>
-      </c>
-      <c r="F5" s="9">
-        <v>200</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>167</v>
+        <v>162</v>
+      </c>
+      <c r="J3" s="14">
+        <v>44955</v>
+      </c>
+      <c r="K3" s="14">
+        <v>45109</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="sSeu3QEkHpXamCixFkV5bs9F0DcFuwrd0kJBGeaMW3s2G45a2FS8UoN2VJrqJQjW/sKLc0ApK/wsUHTGYZuMlA==" saltValue="JMBwYyFdYM1WMhHqfHr2+w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="SAKgLZ9XXq8LfIgS21D4f25/4C9k5FB1hiYKEcIsz/W7/yj4r6I3Y3GyHG/UDaib2xcxDMfOcDfMzUO4r1KOlQ==" saltValue="8gwJyNeyDhOZWB00bkEKUw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="D3:D1048576">
     <cfRule type="expression" dxfId="3" priority="2">
@@ -1346,12 +1338,12 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:E1048576 D1:E1">
     <cfRule type="expression" dxfId="2" priority="3">
-      <formula>$C:$C="Total Spend"</formula>
+      <formula>$C$1:$C$1048574="Total Spend"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:G1048576 F1:G1">
     <cfRule type="expression" dxfId="1" priority="5">
-      <formula>$C:$C ="Consumption"</formula>
+      <formula>$C$1:$C$1048574 ="Consumption"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:G1048576">
@@ -1360,25 +1352,25 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C505:C1048576" xr:uid="{E8E9EA8B-F502-456B-8568-B3A4675F91E0}">
+      <formula1>"Consumption ,Total Spend"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C505:C1048576 B3:B1048576" xr:uid="{29F60392-3D0B-4EB3-94E7-4C10F24024C2}">
+      <formula1>2020</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H1048576" xr:uid="{F8764847-9C39-4CD8-A2DB-642B0361E72F}">
       <formula1>"estimated, actual"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C507:C1048576" xr:uid="{E8E9EA8B-F502-456B-8568-B3A4675F91E0}">
-      <formula1>"Consumption ,Total Spend"</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B1048576 C507:C1048576" xr:uid="{29F60392-3D0B-4EB3-94E7-4C10F24024C2}">
-      <formula1>2020</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E1048576" xr:uid="{06635ADA-7664-4747-91AB-2EB240994011}">
       <formula1>"Onsite heat and steam,District heat and steam"</formula1>
     </dataValidation>
-    <dataValidation type="custom" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D1048576" xr:uid="{9DEC22D6-A9B9-4942-B6B3-A759EF71BB17}">
-      <formula1>$C5 = "Consumption "</formula1>
+    <dataValidation type="custom" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D1048576" xr:uid="{9DEC22D6-A9B9-4942-B6B3-A759EF71BB17}">
+      <formula1>$C4 = "Consumption "</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F1048576" xr:uid="{A931B69C-F657-4E55-A7D7-D60577855578}">
-      <formula1>$C6 = "Total Spend"</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F1048576" xr:uid="{A931B69C-F657-4E55-A7D7-D60577855578}">
+      <formula1>$C4 = "Total Spend"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C506" xr:uid="{CDCAB257-5342-49DF-8EB4-488354E670D6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C504" xr:uid="{CDCAB257-5342-49DF-8EB4-488354E670D6}">
       <formula1>"Total Spend, Consumption"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3351,6 +3343,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100316A6B2706F22F479EB96B4E836A2AA9" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="eb14f50e3c0e0698014ac1b2b11cfd92">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="952decf2-c70e-41dd-b7af-a901e5274ebc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8e289b93c4a0db376190258ac9ef1386" ns3:_="">
     <xsd:import namespace="952decf2-c70e-41dd-b7af-a901e5274ebc"/>
@@ -3506,15 +3507,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5CB81E96-B275-45CD-95A3-7CAF8501621C}">
   <ds:schemaRefs>
@@ -3526,6 +3518,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{030898A3-B818-4BF2-B335-BCA1316059E0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91CA701E-F7B0-428B-9668-E44388524238}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3541,12 +3541,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{030898A3-B818-4BF2-B335-BCA1316059E0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>